<commit_message>
reexport 50% tranzit 10%
</commit_message>
<xml_diff>
--- a/src/main/resources/BlancRe.xlsx
+++ b/src/main/resources/BlancRe.xlsx
@@ -588,7 +588,7 @@
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:AD1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>

</xml_diff>